<commit_message>
J'ai add su stock ?
</commit_message>
<xml_diff>
--- a/Squelette_sujet_TEST/Squelette_sujet_TEST.xlsx
+++ b/Squelette_sujet_TEST/Squelette_sujet_TEST.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="80">
   <si>
     <t>Stimulus</t>
   </si>
@@ -241,6 +241,18 @@
   </si>
   <si>
     <t>ERREUR</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_Test_1</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_Test_2</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_Test_3</t>
+  </si>
+  <si>
+    <t>Squelette_sujet_Test_4</t>
   </si>
 </sst>
 </file>
@@ -261,7 +273,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -271,14 +283,18 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -291,157 +307,157 @@
   <dimension ref="A1:I35"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="true"/>
+    <col min="1" max="1" width="22" customWidth="true"/>
     <col min="2" max="2" width="17" customWidth="true"/>
     <col min="3" max="3" width="10" customWidth="true"/>
     <col min="4" max="4" width="18.85546875" customWidth="true"/>
     <col min="5" max="5" width="11.85546875" customWidth="true"/>
-    <col min="6" max="6" width="13.7109375" customWidth="true"/>
+    <col min="6" max="6" width="12.7109375" customWidth="true"/>
     <col min="7" max="7" width="6.42578125" customWidth="true"/>
     <col min="8" max="8" width="11.7109375" customWidth="true"/>
-    <col min="9" max="9" width="7.85546875" customWidth="true"/>
+    <col min="9" max="9" width="6.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2">
+        <v>1.0783318998292089</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3">
+        <v>0.22487019980326295</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" t="b">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2">
-        <v>0.45330760022625327</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="C4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4">
+        <v>0.31397949997335672</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3">
-        <v>0.25114750023931265</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4">
-        <v>0.20812499988824129</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="H4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>46</v>
+      <c r="A5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="F5">
-        <v>0.062201600056141615</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>0.52217360027134418</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="H5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>

</xml_diff>